<commit_message>
Modified the IRGA conversion script output to select just the columns I want. These must be the FINAL modifications to these spreadsheets; hereafter they are manually edited.
</commit_message>
<xml_diff>
--- a/data/IRGA_flux/manual_files/2022_179_IRGA_WILL.xlsx
+++ b/data/IRGA_flux/manual_files/2022_179_IRGA_WILL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/declantaylor/Documents/Work/Henry_Lab/Alex2022/honours_thesis/data/IRGA_flux/manual_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3F2795-800A-4E46-8739-2E1251DA097B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA2FA44-380C-744D-939B-1DDCA642843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{A65948C4-7519-2C49-A61D-ED674D231560}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{A65948C4-7519-2C49-A61D-ED674D231560}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,8 +447,8 @@
   <dimension ref="A1:Q983"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A936" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K983" sqref="K983"/>
+      <pane ySplit="1" topLeftCell="A932" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P937" sqref="P937"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,10 +500,10 @@
         <v>13</v>
       </c>
       <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
         <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>